<commit_message>
20210908 2240 tlw87 EOD updates.
</commit_message>
<xml_diff>
--- a/docs/AMT-mvc.xlsx
+++ b/docs/AMT-mvc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\amt-mvc\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\amt-mvc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECD54FF-D6B5-4771-80C1-E973F9DA90EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15530" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="RTM" sheetId="3" r:id="rId3"/>
     <sheet name="States" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="300">
   <si>
     <t>Test Class</t>
   </si>
@@ -994,12 +995,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
     <numFmt numFmtId="165" formatCode="000.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1543,7 +1544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1551,19 +1552,19 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="83.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="141.26953125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="141.28515625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>138</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <v>1</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <f>A2+1</f>
         <v>2</v>
@@ -1642,7 +1643,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <f t="shared" ref="A4:A31" si="0">A3+1</f>
         <v>3</v>
@@ -1669,7 +1670,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1696,7 +1697,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1723,7 +1724,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1750,7 +1751,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1777,7 +1778,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1804,7 +1805,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1831,7 +1832,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1858,7 +1859,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1885,7 +1886,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1912,7 +1913,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1939,7 +1940,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1966,7 +1967,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1993,7 +1994,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2020,7 +2021,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2047,7 +2048,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2074,7 +2075,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2101,7 +2102,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="34">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2128,7 +2129,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="34">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2155,7 +2156,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="34">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2182,7 +2183,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="34">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2209,7 +2210,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="34">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2236,7 +2237,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="34">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2263,7 +2264,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="34">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2290,7 +2291,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="34">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2317,7 +2318,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="34">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2344,7 +2345,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2371,7 +2372,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="34">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2405,31 +2406,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
-    <col min="4" max="4" width="27.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.26953125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="27.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -2458,7 +2459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -2479,7 +2480,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -2502,7 +2503,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
@@ -2515,7 +2516,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>8</v>
@@ -2528,7 +2529,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>8</v>
@@ -2541,7 +2542,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>8</v>
@@ -2554,7 +2555,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="21"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>8</v>
@@ -2567,7 +2568,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>8</v>
@@ -2580,7 +2581,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
@@ -2593,7 +2594,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
         <v>8</v>
@@ -2606,7 +2607,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="38"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>8</v>
@@ -2619,7 +2620,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="38"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>8</v>
@@ -2632,7 +2633,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>8</v>
@@ -2645,7 +2646,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>8</v>
@@ -2658,7 +2659,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="38"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
         <v>8</v>
@@ -2671,7 +2672,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="38"/>
     </row>
-    <row r="17" spans="1:9" hidden="1">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>8</v>
@@ -2684,7 +2685,7 @@
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
         <v>8</v>
@@ -2697,7 +2698,7 @@
       <c r="H18" s="18"/>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" hidden="1">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
         <v>8</v>
@@ -2710,7 +2711,7 @@
       <c r="H19" s="18"/>
       <c r="I19" s="38"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
         <v>8</v>
@@ -2723,7 +2724,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
         <v>8</v>
@@ -2736,7 +2737,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
         <v>8</v>
@@ -2749,7 +2750,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
         <v>8</v>
@@ -2762,7 +2763,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>8</v>
@@ -2775,7 +2776,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
         <v>8</v>
@@ -2788,7 +2789,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="38"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
         <v>8</v>
@@ -2801,7 +2802,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>8</v>
@@ -2814,7 +2815,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="38"/>
     </row>
-    <row r="28" spans="1:9" ht="58">
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>1</v>
       </c>
@@ -2837,7 +2838,7 @@
       <c r="H28" s="18"/>
       <c r="I28" s="38"/>
     </row>
-    <row r="29" spans="1:9" ht="58">
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>1.01</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="58">
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>1.01</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="6" customFormat="1" ht="58">
+    <row r="31" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>2</v>
       </c>
@@ -2910,7 +2911,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9" ht="58">
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>2.0099999999999998</v>
       </c>
@@ -2933,7 +2934,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="38"/>
     </row>
-    <row r="33" spans="1:9" s="6" customFormat="1">
+    <row r="33" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15" t="s">
         <v>12</v>
@@ -2946,7 +2947,7 @@
       <c r="H33" s="18"/>
       <c r="I33" s="18"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="15" t="s">
         <v>12</v>
@@ -2959,7 +2960,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="38"/>
     </row>
-    <row r="35" spans="1:9" ht="58">
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>3</v>
       </c>
@@ -2982,7 +2983,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" ht="58">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>4</v>
       </c>
@@ -3005,7 +3006,7 @@
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" ht="101.5">
+    <row r="37" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>5</v>
       </c>
@@ -3028,7 +3029,7 @@
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" ht="116">
+    <row r="38" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>10</v>
       </c>
@@ -3051,7 +3052,7 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" ht="58">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>12</v>
       </c>
@@ -3074,7 +3075,7 @@
       <c r="H39" s="18"/>
       <c r="I39" s="38"/>
     </row>
-    <row r="40" spans="1:9" ht="203">
+    <row r="40" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>15</v>
       </c>
@@ -3097,7 +3098,7 @@
       <c r="H40" s="18"/>
       <c r="I40" s="38"/>
     </row>
-    <row r="41" spans="1:9" ht="29">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>15.01</v>
       </c>
@@ -3118,7 +3119,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" ht="217.5">
+    <row r="42" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>20</v>
       </c>
@@ -3141,7 +3142,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" s="6" customFormat="1">
+    <row r="43" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="15" t="s">
         <v>12</v>
@@ -3154,7 +3155,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="18"/>
     </row>
-    <row r="44" spans="1:9" s="6" customFormat="1">
+    <row r="44" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="15" t="s">
         <v>12</v>
@@ -3167,7 +3168,7 @@
       <c r="H44" s="18"/>
       <c r="I44" s="18"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="16" t="s">
         <v>13</v>
@@ -3180,7 +3181,7 @@
       <c r="H45" s="18"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="16" t="s">
         <v>13</v>
@@ -3193,7 +3194,7 @@
       <c r="H46" s="18"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="16" t="s">
         <v>13</v>
@@ -3206,7 +3207,7 @@
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="17" t="s">
         <v>14</v>
@@ -3219,7 +3220,7 @@
       <c r="H48" s="18"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="17" t="s">
         <v>14</v>
@@ -3232,7 +3233,7 @@
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="17" t="s">
         <v>14</v>
@@ -3245,7 +3246,7 @@
       <c r="H50" s="18"/>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="17" t="s">
         <v>14</v>
@@ -3258,7 +3259,7 @@
       <c r="H51" s="18"/>
       <c r="I51" s="18"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="17" t="s">
         <v>14</v>
@@ -3271,7 +3272,7 @@
       <c r="H52" s="18"/>
       <c r="I52" s="19"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -3282,7 +3283,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -3293,7 +3294,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -3304,7 +3305,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -3315,7 +3316,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -3326,7 +3327,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -3337,7 +3338,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -3348,7 +3349,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -3359,7 +3360,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -3370,7 +3371,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -3381,7 +3382,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -3392,7 +3393,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -3403,7 +3404,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -3414,7 +3415,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
@@ -3425,7 +3426,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
@@ -3436,7 +3437,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
@@ -3447,7 +3448,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
@@ -3458,7 +3459,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
@@ -3469,7 +3470,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
@@ -3480,7 +3481,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
@@ -3491,7 +3492,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
@@ -3502,7 +3503,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
@@ -3513,7 +3514,7 @@
       <c r="H74" s="12"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
@@ -3531,7 +3532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3539,19 +3540,19 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="75.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7265625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="35.453125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="26" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>60</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>61</v>
       </c>
@@ -3603,7 +3604,7 @@
       </c>
       <c r="I2" s="31"/>
     </row>
-    <row r="3" spans="1:9" ht="29">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>61</v>
       </c>
@@ -3628,7 +3629,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>61</v>
       </c>
@@ -3651,7 +3652,7 @@
       </c>
       <c r="I4" s="31"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>61</v>
       </c>
@@ -3674,7 +3675,7 @@
       </c>
       <c r="I5" s="31"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>61</v>
       </c>
@@ -3695,7 +3696,7 @@
       </c>
       <c r="I6" s="31"/>
     </row>
-    <row r="7" spans="1:9" ht="29">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>61</v>
       </c>
@@ -3716,7 +3717,7 @@
       </c>
       <c r="I7" s="31"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>61</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>61</v>
       </c>
@@ -3760,7 +3761,7 @@
       </c>
       <c r="I9" s="31"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>61</v>
       </c>
@@ -3779,7 +3780,7 @@
       </c>
       <c r="I10" s="31"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>61</v>
       </c>
@@ -3796,7 +3797,7 @@
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>61</v>
       </c>
@@ -3813,7 +3814,7 @@
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>61</v>
       </c>
@@ -3830,7 +3831,7 @@
       <c r="H13" s="31"/>
       <c r="I13" s="31"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>61</v>
       </c>
@@ -3851,7 +3852,7 @@
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>61</v>
       </c>
@@ -3872,7 +3873,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>61</v>
       </c>
@@ -3893,7 +3894,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>61</v>
       </c>
@@ -3914,7 +3915,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>61</v>
       </c>
@@ -3933,7 +3934,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>61</v>
       </c>
@@ -3963,20 +3964,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" thickBot="1">
+    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>148</v>
       </c>
@@ -3984,7 +3985,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" thickBot="1">
+    <row r="2" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>150</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5" thickBot="1">
+    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>152</v>
       </c>
@@ -4000,7 +4001,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" thickBot="1">
+    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>154</v>
       </c>
@@ -4008,7 +4009,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="19.5" thickBot="1">
+    <row r="5" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>156</v>
       </c>
@@ -4016,7 +4017,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="19.5" thickBot="1">
+    <row r="6" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>158</v>
       </c>
@@ -4024,7 +4025,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.5" thickBot="1">
+    <row r="7" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>160</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.5" thickBot="1">
+    <row r="8" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>162</v>
       </c>
@@ -4040,7 +4041,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="19.5" thickBot="1">
+    <row r="9" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>164</v>
       </c>
@@ -4048,7 +4049,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="19.5" thickBot="1">
+    <row r="10" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>166</v>
       </c>
@@ -4056,7 +4057,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="19.5" thickBot="1">
+    <row r="11" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>168</v>
       </c>
@@ -4064,7 +4065,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="19.5" thickBot="1">
+    <row r="12" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>170</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="19.5" thickBot="1">
+    <row r="13" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>172</v>
       </c>
@@ -4080,7 +4081,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19.5" thickBot="1">
+    <row r="14" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>174</v>
       </c>
@@ -4088,7 +4089,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="19.5" thickBot="1">
+    <row r="15" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
         <v>176</v>
       </c>
@@ -4096,7 +4097,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="19.5" thickBot="1">
+    <row r="16" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>178</v>
       </c>
@@ -4104,7 +4105,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="19.5" thickBot="1">
+    <row r="17" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>180</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="19.5" thickBot="1">
+    <row r="18" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35" t="s">
         <v>182</v>
       </c>
@@ -4120,7 +4121,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="19.5" thickBot="1">
+    <row r="19" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35" t="s">
         <v>184</v>
       </c>
@@ -4128,7 +4129,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="19.5" thickBot="1">
+    <row r="20" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35" t="s">
         <v>186</v>
       </c>
@@ -4136,7 +4137,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="19.5" thickBot="1">
+    <row r="21" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
         <v>188</v>
       </c>
@@ -4144,7 +4145,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="19.5" thickBot="1">
+    <row r="22" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>190</v>
       </c>
@@ -4152,7 +4153,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="19.5" thickBot="1">
+    <row r="23" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35" t="s">
         <v>192</v>
       </c>
@@ -4160,7 +4161,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="19.5" thickBot="1">
+    <row r="24" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
         <v>194</v>
       </c>
@@ -4168,7 +4169,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="19.5" thickBot="1">
+    <row r="25" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>196</v>
       </c>
@@ -4176,7 +4177,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="19.5" thickBot="1">
+    <row r="26" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35" t="s">
         <v>198</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="19.5" thickBot="1">
+    <row r="27" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
         <v>200</v>
       </c>
@@ -4192,7 +4193,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="19.5" thickBot="1">
+    <row r="28" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35" t="s">
         <v>202</v>
       </c>
@@ -4200,7 +4201,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="19.5" thickBot="1">
+    <row r="29" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="35" t="s">
         <v>204</v>
       </c>
@@ -4208,7 +4209,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="19.5" thickBot="1">
+    <row r="30" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35" t="s">
         <v>206</v>
       </c>
@@ -4216,7 +4217,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="19.5" thickBot="1">
+    <row r="31" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>208</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="19.5" thickBot="1">
+    <row r="32" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>210</v>
       </c>
@@ -4232,7 +4233,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="19.5" thickBot="1">
+    <row r="33" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>212</v>
       </c>
@@ -4240,7 +4241,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="19.5" thickBot="1">
+    <row r="34" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>214</v>
       </c>
@@ -4248,7 +4249,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="19.5" thickBot="1">
+    <row r="35" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>216</v>
       </c>
@@ -4256,7 +4257,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="19.5" thickBot="1">
+    <row r="36" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>218</v>
       </c>
@@ -4264,7 +4265,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="19.5" thickBot="1">
+    <row r="37" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>220</v>
       </c>
@@ -4272,7 +4273,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="19.5" thickBot="1">
+    <row r="38" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="35" t="s">
         <v>222</v>
       </c>
@@ -4280,7 +4281,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="19.5" thickBot="1">
+    <row r="39" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>224</v>
       </c>
@@ -4288,7 +4289,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="19.5" thickBot="1">
+    <row r="40" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>226</v>
       </c>
@@ -4296,7 +4297,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="19.5" thickBot="1">
+    <row r="41" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35" t="s">
         <v>228</v>
       </c>
@@ -4304,7 +4305,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="19.5" thickBot="1">
+    <row r="42" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>230</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="19.5" thickBot="1">
+    <row r="43" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35" t="s">
         <v>232</v>
       </c>
@@ -4320,7 +4321,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="19.5" thickBot="1">
+    <row r="44" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
         <v>234</v>
       </c>
@@ -4328,7 +4329,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="19.5" thickBot="1">
+    <row r="45" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
         <v>236</v>
       </c>
@@ -4336,7 +4337,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="19.5" thickBot="1">
+    <row r="46" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>238</v>
       </c>
@@ -4344,7 +4345,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="19.5" thickBot="1">
+    <row r="47" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>240</v>
       </c>
@@ -4352,7 +4353,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="19.5" thickBot="1">
+    <row r="48" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>242</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="19.5" thickBot="1">
+    <row r="49" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="35" t="s">
         <v>244</v>
       </c>
@@ -4368,7 +4369,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="19.5" thickBot="1">
+    <row r="50" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="35" t="s">
         <v>246</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="19.5" thickBot="1">
+    <row r="51" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="35" t="s">
         <v>248</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="19.5" thickBot="1">
+    <row r="52" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>250</v>
       </c>
@@ -4392,7 +4393,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="19.5" thickBot="1">
+    <row r="53" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>252</v>
       </c>
@@ -4400,7 +4401,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="19.5" thickBot="1">
+    <row r="54" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35" t="s">
         <v>254</v>
       </c>
@@ -4408,7 +4409,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="19.5" thickBot="1">
+    <row r="55" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="35" t="s">
         <v>256</v>
       </c>
@@ -4416,7 +4417,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="19">
+    <row r="56" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
         <v>258</v>
       </c>

</xml_diff>